<commit_message>
Correct definition of the CO2 backstop process
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SYS_OtherNewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SYS_OtherNewTechs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\times-ireland-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36338BDC-C2C4-47A0-9D7E-EB7799F5A5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3787F6-9A9C-46C3-A80F-A2A9712881B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15390" windowHeight="9443" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -137,53 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This attribute is used for Combined Heat and Power Technologies
-By defautt is defined like fixed share  </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>FX</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">.
-If you want upper or lower add
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>~UP
- ~LO</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B14" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -297,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -370,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -454,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -507,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -540,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -633,7 +587,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -696,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1735,7 +1689,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="107">
   <si>
     <t>~FI_T</t>
   </si>
@@ -1878,15 +1832,6 @@
     <t>Output Commodity</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>AFA</t>
-  </si>
-  <si>
     <t>VAROM</t>
   </si>
   <si>
@@ -1896,15 +1841,6 @@
     <t>Efficiency</t>
   </si>
   <si>
-    <t>Fuel input level</t>
-  </si>
-  <si>
-    <t>Fuel Output level</t>
-  </si>
-  <si>
-    <t>Annual Availability Factor</t>
-  </si>
-  <si>
     <t>Lifetime of Process</t>
   </si>
   <si>
@@ -2049,10 +1985,31 @@
     <t>Specify hydrogen import and DACS (backstop) technology</t>
   </si>
   <si>
-    <t>*CO2*, -*CO2S</t>
-  </si>
-  <si>
     <t>MEUR2020</t>
+  </si>
+  <si>
+    <t>AGRCO2N</t>
+  </si>
+  <si>
+    <t>INDCO2N</t>
+  </si>
+  <si>
+    <t>INDCO2P</t>
+  </si>
+  <si>
+    <t>PWRCO2N</t>
+  </si>
+  <si>
+    <t>RSDCO2</t>
+  </si>
+  <si>
+    <t>SRVCO2N</t>
+  </si>
+  <si>
+    <t>SUPCO2N</t>
+  </si>
+  <si>
+    <t>TRACO2N</t>
   </si>
 </sst>
 </file>
@@ -3156,7 +3113,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3596,7 +3553,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="32" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -3682,10 +3639,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -3714,10 +3671,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -3746,10 +3703,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -3806,10 +3763,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
@@ -3839,7 +3796,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="23"/>
       <c r="B24" s="26" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -3869,7 +3826,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="23"/>
       <c r="B25" s="26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -3898,10 +3855,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
@@ -3986,7 +3943,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="23" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B29" s="27">
         <v>1</v>
@@ -4018,10 +3975,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="23" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31"/>
@@ -4050,10 +4007,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="23" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -4083,7 +4040,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="29"/>
       <c r="B32" s="30" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
@@ -6009,55 +5966,45 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:X35"/>
+  <dimension ref="B1:R40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.86328125" customWidth="1"/>
-    <col min="2" max="2" width="40.73046875" customWidth="1"/>
-    <col min="3" max="3" width="22.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.86328125" customWidth="1"/>
-    <col min="6" max="6" width="15.1328125" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.86328125" customWidth="1"/>
-    <col min="8" max="8" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.3984375" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="13" width="13.1328125" customWidth="1"/>
-    <col min="14" max="14" width="9.86328125" customWidth="1"/>
-    <col min="15" max="15" width="13.1328125" customWidth="1"/>
-    <col min="16" max="16" width="11.265625" customWidth="1"/>
-    <col min="17" max="17" width="12.59765625" customWidth="1"/>
-    <col min="18" max="18" width="14.59765625" customWidth="1"/>
-    <col min="19" max="19" width="13.1328125" customWidth="1"/>
-    <col min="20" max="20" width="13.86328125" customWidth="1"/>
-    <col min="21" max="21" width="11.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.86328125" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" customWidth="1"/>
+    <col min="12" max="12" width="11.265625" customWidth="1"/>
+    <col min="13" max="13" width="12.59765625" customWidth="1"/>
+    <col min="14" max="14" width="13.86328125" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:16" ht="17.25" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="2:24" ht="13.15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="2:16" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>4</v>
@@ -6071,44 +6018,20 @@
       <c r="G2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="2:24" s="2" customFormat="1" ht="38.65" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="2:16" s="2" customFormat="1" ht="38.65" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="11" t="s">
         <v>42</v>
       </c>
@@ -6128,410 +6051,378 @@
         <v>46</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="11" t="s">
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" t="str">
+        <f>C23</f>
+        <v>SCO2DACS</v>
+      </c>
+      <c r="C4" t="str">
+        <f>D23</f>
+        <v>CO2 Backstop process</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="20" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="2:18" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="B21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="38.65" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-    </row>
-    <row r="4" spans="2:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" t="str">
-        <f>C18</f>
-        <v>SCO2DACS</v>
-      </c>
-      <c r="C4" t="str">
-        <f>D18</f>
-        <v>CO2 Backstop process</v>
-      </c>
-      <c r="E4" t="s">
-        <v>104</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:24" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="2:24" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:24" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="15" spans="2:24" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="2:24" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:24" ht="38.65" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="I26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="I27" s="14"/>
-      <c r="M27" s="14"/>
+      <c r="F23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
       <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="I28" s="14"/>
-      <c r="M28" s="14"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
       <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
       <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="I29" s="14"/>
-      <c r="M29" s="14"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="I30" s="14"/>
-      <c r="M30" s="14"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
       <c r="N30" s="14"/>
       <c r="O30" s="14"/>
       <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
       <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="14"/>
-      <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
-      <c r="X30" s="14"/>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
       <c r="I31" s="14"/>
-      <c r="M31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
       <c r="N31" s="14"/>
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="14"/>
-      <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
       <c r="I32" s="14"/>
-      <c r="M32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
       <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
       <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="14"/>
-      <c r="V32" s="14"/>
-      <c r="W32" s="14"/>
-      <c r="X32" s="14"/>
-    </row>
-    <row r="33" spans="9:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="9:18" x14ac:dyDescent="0.35">
       <c r="I33" s="14"/>
-      <c r="M33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>
       <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-      <c r="V33" s="14"/>
-      <c r="W33" s="14"/>
-      <c r="X33" s="14"/>
-    </row>
-    <row r="34" spans="9:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="9:18" x14ac:dyDescent="0.35">
       <c r="I34" s="14"/>
-      <c r="M34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="14"/>
-      <c r="W34" s="14"/>
-      <c r="X34" s="14"/>
-    </row>
-    <row r="35" spans="9:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="9:18" x14ac:dyDescent="0.35">
       <c r="I35" s="14"/>
-      <c r="M35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
       <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="14"/>
-      <c r="V35" s="14"/>
-      <c r="W35" s="14"/>
-      <c r="X35" s="14"/>
+    </row>
+    <row r="36" spans="9:18" x14ac:dyDescent="0.35">
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+    </row>
+    <row r="37" spans="9:18" x14ac:dyDescent="0.35">
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+    </row>
+    <row r="38" spans="9:18" x14ac:dyDescent="0.35">
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+    </row>
+    <row r="39" spans="9:18" x14ac:dyDescent="0.35">
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+    </row>
+    <row r="40" spans="9:18" x14ac:dyDescent="0.35">
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -6570,7 +6461,7 @@
   <sheetData>
     <row r="1" spans="2:18" ht="17.25" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1"/>
       <c r="H1" s="3" t="s">
@@ -6584,7 +6475,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>3</v>
@@ -6593,13 +6484,13 @@
         <v>5</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>17</v>
@@ -6608,28 +6499,28 @@
         <v>19</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="N2" s="13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="64.150000000000006" thickBot="1" x14ac:dyDescent="0.4">
@@ -6650,37 +6541,37 @@
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
@@ -6697,16 +6588,16 @@
         <v/>
       </c>
       <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
         <v>72</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
       </c>
       <c r="G4">
         <v>2030</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I4">
         <v>2025</v>
@@ -6721,16 +6612,16 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
         <v>72</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
       </c>
       <c r="G5">
         <v>2050</v>
       </c>
       <c r="H5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K5">
         <f>6*2</f>
@@ -6871,19 +6762,19 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>

</xml_diff>